<commit_message>
updated benchmark and figures
</commit_message>
<xml_diff>
--- a/figures/supplement/benchmark_class_counts/benchmark_class_counts.xlsx
+++ b/figures/supplement/benchmark_class_counts/benchmark_class_counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackson/Dropbox (MIT)/work/07-SLiM_bioinformatics/07-pt1_pt2_combined/figures/supplement/benchmark_class_counts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackson/Dropbox (MIT)/work/07-SLiM_bioinformatics/08-benchmark/figures/supplement/benchmark_class_counts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4FE58C3-D041-1D4E-8D92-50AFCE4EB205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A9D0043-8E35-2747-A805-5C9350F8EF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{F1D60101-47FD-7243-80BB-8B11063D8D1A}"/>
+    <workbookView xWindow="19200" yWindow="520" windowWidth="19180" windowHeight="21060" xr2:uid="{BDF10DF6-A4EA-F64A-8B3C-78AFA849E4C1}"/>
   </bookViews>
   <sheets>
     <sheet name="benchmark_class_counts" sheetId="1" r:id="rId1"/>
@@ -94,16 +94,16 @@
     <t>[0 0 0 1 0 1 0 0 1]</t>
   </si>
   <si>
+    <t>motif regular expression</t>
+  </si>
+  <si>
+    <t>true positives</t>
+  </si>
+  <si>
+    <t>background</t>
+  </si>
+  <si>
     <t>motif</t>
-  </si>
-  <si>
-    <t>background</t>
-  </si>
-  <si>
-    <t>true positives</t>
-  </si>
-  <si>
-    <t>motif regular expression</t>
   </si>
   <si>
     <t>mask</t>
@@ -113,25 +113,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Aptos Display"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -139,7 +139,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -147,7 +147,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -155,98 +155,104 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -590,8 +596,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -661,39 +668,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -745,7 +752,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -856,6 +863,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -864,13 +878,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -935,58 +942,38 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8221846F-1DB6-4748-AEC8-B41EFC02E9FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260A5BED-7644-DE44-92AF-DD707BC4AF0E}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>28</v>
@@ -997,10 +984,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="C2">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1014,7 +1001,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C3">
         <v>34</v>
@@ -1031,10 +1018,10 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1048,7 +1035,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C5">
         <v>49</v>
@@ -1065,7 +1052,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C6">
         <v>49</v>
@@ -1082,7 +1069,7 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>210</v>
+        <v>238</v>
       </c>
       <c r="C7">
         <v>18</v>
@@ -1099,7 +1086,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="C8">
         <v>28</v>
@@ -1116,7 +1103,7 @@
         <v>21</v>
       </c>
       <c r="B9">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="C9">
         <v>7</v>

</xml_diff>